<commit_message>
Log and feature selection is applied
</commit_message>
<xml_diff>
--- a/Data_Learning_Prediction/Tuned_Parameters.xlsx
+++ b/Data_Learning_Prediction/Tuned_Parameters.xlsx
@@ -9,22 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="10548" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RF" sheetId="1" r:id="rId1"/>
     <sheet name="NN" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NN!$A$1:$Q$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RF!$A$1:$S$10</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="71">
   <si>
     <t>Datetime</t>
   </si>
@@ -41,6 +37,9 @@
     <t>Product</t>
   </si>
   <si>
+    <t>dependenttype</t>
+  </si>
+  <si>
     <t>est</t>
   </si>
   <si>
@@ -92,34 +91,64 @@
     <t>auto</t>
   </si>
   <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>01-05 07:48</t>
+  </si>
+  <si>
+    <t>CHN</t>
+  </si>
+  <si>
+    <t>01-05 08:08</t>
+  </si>
+  <si>
+    <t>02-10 19:14</t>
+  </si>
+  <si>
+    <t>_345</t>
+  </si>
+  <si>
     <t>01-04 17:28</t>
   </si>
   <si>
-    <t>CHN</t>
-  </si>
-  <si>
-    <t>01-05 07:48</t>
-  </si>
-  <si>
-    <t>01-05 08:08</t>
-  </si>
-  <si>
     <t>01-05 08:37</t>
   </si>
   <si>
+    <t>01-05 09:13</t>
+  </si>
+  <si>
+    <t>01-06 07:48</t>
+  </si>
+  <si>
+    <t>02-11 15:19</t>
+  </si>
+  <si>
     <t>01-05 08:48</t>
   </si>
   <si>
-    <t>01-05 09:13</t>
-  </si>
-  <si>
-    <t>01-06 07:48</t>
-  </si>
-  <si>
-    <t>02-10 19:14</t>
-  </si>
-  <si>
-    <t>_345</t>
+    <t>02-11 21:54</t>
+  </si>
+  <si>
+    <t>02-13 12:17</t>
+  </si>
+  <si>
+    <t>_45</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>02-14 17:06</t>
+  </si>
+  <si>
+    <t>_234</t>
+  </si>
+  <si>
+    <t>02-14 17:18</t>
+  </si>
+  <si>
+    <t>_34</t>
   </si>
   <si>
     <t>Solver</t>
@@ -186,6 +215,24 @@
   </si>
   <si>
     <t>02-10 19:18</t>
+  </si>
+  <si>
+    <t>02-11 15:22</t>
+  </si>
+  <si>
+    <t>02-11 21:57</t>
+  </si>
+  <si>
+    <t>02-13 12:11</t>
+  </si>
+  <si>
+    <t>(30, 100, 30)</t>
+  </si>
+  <si>
+    <t>02-14 17:09</t>
+  </si>
+  <si>
+    <t>02-14 17:27</t>
   </si>
 </sst>
 </file>
@@ -548,15 +595,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,19 +661,22 @@
       <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -631,211 +684,226 @@
       <c r="F2">
         <v>841810</v>
       </c>
-      <c r="H2">
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="I2">
         <v>0.75700000000000001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.75849999999999995</v>
       </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2">
         <v>200</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.01</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.76200000000000001</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.76300000000000001</v>
       </c>
-      <c r="R2">
-        <v>100</v>
-      </c>
-      <c r="S2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
-        <v>841840</v>
-      </c>
-      <c r="H3">
-        <v>0.55800000000000005</v>
+        <v>841810</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
       </c>
       <c r="I3">
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3">
-        <v>300</v>
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="J3">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
       <c r="L3">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="N3">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
         <v>1E-4</v>
       </c>
-      <c r="P3">
-        <v>0.56499999999999995</v>
-      </c>
       <c r="Q3">
-        <v>0.57299999999999995</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="R3">
-        <v>100</v>
-      </c>
-      <c r="S3">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="S3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>841810</v>
       </c>
-      <c r="H4">
-        <v>0.64600000000000002</v>
+      <c r="G4">
+        <v>100</v>
       </c>
       <c r="I4">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="J4">
+        <v>0.57299999999999995</v>
       </c>
       <c r="K4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="O4">
-        <v>1E-4</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0.64700000000000002</v>
+        <v>1E-3</v>
       </c>
       <c r="Q4">
-        <v>0.66100000000000003</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="R4">
-        <v>100</v>
-      </c>
-      <c r="S4">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="S4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
       </c>
       <c r="F5">
         <v>841810</v>
       </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
       <c r="H5">
-        <v>0.56699999999999995</v>
+        <v>500</v>
       </c>
       <c r="I5">
-        <v>0.57299999999999995</v>
+        <v>0.66</v>
       </c>
       <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
       </c>
       <c r="L5">
-        <v>9.9999999999999995E-7</v>
+        <v>200</v>
+      </c>
+      <c r="M5">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
-      <c r="O5">
-        <v>1E-3</v>
-      </c>
       <c r="P5">
-        <v>0.56799999999999995</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q5">
-        <v>0.57399999999999995</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="R5">
-        <v>100</v>
-      </c>
-      <c r="S5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="S5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -843,105 +911,111 @@
       <c r="F6">
         <v>841840</v>
       </c>
-      <c r="H6">
-        <v>0.56100000000000005</v>
+      <c r="G6">
+        <v>100</v>
       </c>
       <c r="I6">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6">
-        <v>100</v>
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="J6">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
       </c>
       <c r="L6">
+        <v>300</v>
+      </c>
+      <c r="M6">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>5</v>
       </c>
-      <c r="O6">
-        <v>1E-3</v>
-      </c>
       <c r="P6">
-        <v>0.55900000000000005</v>
+        <v>1E-4</v>
       </c>
       <c r="Q6">
         <v>0.56499999999999995</v>
       </c>
       <c r="R6">
-        <v>100</v>
-      </c>
-      <c r="S6">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="S6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="F7">
-        <v>841850</v>
-      </c>
-      <c r="H7">
-        <v>0.88900000000000001</v>
+        <v>841840</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
       </c>
       <c r="I7">
-        <v>0.89</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="J7">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>300</v>
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
       </c>
       <c r="L7">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="M7">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="O7">
         <v>5</v>
       </c>
-      <c r="O7">
-        <v>0.01</v>
-      </c>
       <c r="P7">
-        <v>0.89200000000000002</v>
+        <v>1E-3</v>
       </c>
       <c r="Q7">
-        <v>0.89400000000000002</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="R7">
-        <v>100</v>
-      </c>
-      <c r="S7">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="S7" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -949,52 +1023,55 @@
       <c r="F8">
         <v>841850</v>
       </c>
-      <c r="H8">
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="I8">
         <v>0.76200000000000001</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>10</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>100</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>1</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.01</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.76</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.76400000000000001</v>
       </c>
-      <c r="R8">
-        <v>100</v>
-      </c>
-      <c r="S8">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1003,118 +1080,410 @@
         <v>841840</v>
       </c>
       <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
         <v>1000</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.113</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.11600000000000001</v>
-      </c>
-      <c r="J9">
-        <v>10</v>
       </c>
       <c r="K9">
         <v>10</v>
       </c>
       <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.01</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>0.111</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.115</v>
       </c>
-      <c r="R9">
+      <c r="S9" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>841840</v>
+      </c>
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="S9">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="H10">
+        <v>200</v>
+      </c>
+      <c r="I10">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="J10">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>1E-4</v>
+      </c>
+      <c r="Q10">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="R10">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="S10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10">
+      <c r="T10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>841850</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="J11">
+        <v>0.89</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>300</v>
+      </c>
+      <c r="M11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <v>0.01</v>
+      </c>
+      <c r="Q11">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="R11">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="S11" t="s">
+        <v>23</v>
+      </c>
+      <c r="T11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>841850</v>
+      </c>
+      <c r="G12">
+        <v>75</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <v>300</v>
+      </c>
+      <c r="M12">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>1E-3</v>
+      </c>
+      <c r="Q12">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="R12">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="S12" t="s">
+        <v>23</v>
+      </c>
+      <c r="T12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>841840</v>
+      </c>
+      <c r="G13">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>500</v>
+      </c>
+      <c r="I13">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="J13">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13">
+        <v>200</v>
+      </c>
+      <c r="M13">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1E-3</v>
+      </c>
+      <c r="Q13">
+        <v>0.71</v>
+      </c>
+      <c r="R13">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="S13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T13">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14">
         <v>841810</v>
       </c>
-      <c r="G10">
-        <v>500</v>
-      </c>
-      <c r="H10">
-        <v>0.66</v>
-      </c>
-      <c r="I10">
-        <v>0.66400000000000003</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10">
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
         <v>200</v>
       </c>
-      <c r="L10">
+      <c r="I14">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="J14">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M10">
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>1E-3</v>
+      </c>
+      <c r="Q14">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R14">
+        <v>0.74</v>
+      </c>
+      <c r="S14" t="s">
+        <v>38</v>
+      </c>
+      <c r="T14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>841850</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>1000</v>
+      </c>
+      <c r="I15">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="J15">
+        <v>0.93</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <v>200</v>
+      </c>
+      <c r="M15">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="N15">
         <v>1</v>
       </c>
-      <c r="O10">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="P10">
-        <v>0.66300000000000003</v>
-      </c>
-      <c r="Q10">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="R10">
-        <v>50</v>
-      </c>
-      <c r="S10">
-        <v>42</v>
+      <c r="P15">
+        <v>1E-4</v>
+      </c>
+      <c r="Q15">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="R15">
+        <v>0.93</v>
+      </c>
+      <c r="S15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S10"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="17" max="17" width="13.21875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1128,43 +1497,46 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1172,10 +1544,10 @@
         <v>841810</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -1183,41 +1555,44 @@
       <c r="F2">
         <v>100</v>
       </c>
-      <c r="G2">
-        <v>42</v>
-      </c>
-      <c r="H2" t="s">
-        <v>37</v>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2">
         <v>1E-3</v>
       </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2">
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2">
         <v>100000</v>
       </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2">
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2">
         <v>0.77600000000000002</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.77800000000000002</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.75800000000000001</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.77</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1225,10 +1600,10 @@
         <v>841840</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -1236,41 +1611,44 @@
       <c r="F3">
         <v>100</v>
       </c>
-      <c r="G3">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>37</v>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3">
         <v>10000</v>
       </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3">
+      <c r="N3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3">
         <v>0.47799999999999998</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.48</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0.47799999999999998</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.48899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1278,10 +1656,10 @@
         <v>841810</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1289,41 +1667,44 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4">
         <v>1E-3</v>
       </c>
-      <c r="K4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4">
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4">
         <v>50000</v>
       </c>
-      <c r="M4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4">
+      <c r="N4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4">
         <v>0.57699999999999996</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.59399999999999997</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.53800000000000003</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1331,10 +1712,10 @@
         <v>841810</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1342,41 +1723,44 @@
       <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5">
-        <v>42</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5">
+        <v>48</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5">
         <v>1E-3</v>
       </c>
-      <c r="K5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5">
+      <c r="L5" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5">
         <v>100000</v>
       </c>
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5">
+      <c r="N5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5">
         <v>0.52500000000000002</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.52700000000000002</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.52</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -1384,10 +1768,10 @@
         <v>841840</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1395,41 +1779,44 @@
       <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6">
-        <v>42</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6">
         <v>1E-3</v>
       </c>
-      <c r="K6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6">
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6">
         <v>1000</v>
       </c>
-      <c r="M6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6">
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6">
         <v>0.47899999999999998</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.48099999999999998</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.47799999999999998</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.48099999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1437,10 +1824,10 @@
         <v>841850</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1448,41 +1835,44 @@
       <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>37</v>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7">
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7">
         <v>10000</v>
       </c>
-      <c r="M7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7">
+      <c r="N7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7">
         <v>0.84599999999999997</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.84699999999999998</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0.84599999999999997</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1490,10 +1880,10 @@
         <v>841850</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -1501,41 +1891,44 @@
       <c r="F8">
         <v>100</v>
       </c>
-      <c r="G8">
-        <v>42</v>
-      </c>
-      <c r="H8" t="s">
-        <v>37</v>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8">
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8">
         <v>1E-3</v>
       </c>
-      <c r="K8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8">
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8">
         <v>5000</v>
       </c>
-      <c r="M8" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8">
+      <c r="N8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.58299999999999996</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.58899999999999997</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.59299999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1543,10 +1936,10 @@
         <v>841840</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -1554,41 +1947,44 @@
       <c r="F9">
         <v>100</v>
       </c>
-      <c r="G9">
-        <v>42</v>
-      </c>
-      <c r="H9" t="s">
-        <v>37</v>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9">
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9">
+        <v>48</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9">
         <v>1E-3</v>
       </c>
-      <c r="K9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9">
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9">
         <v>1000</v>
       </c>
-      <c r="M9" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9">
+      <c r="N9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9">
         <v>7.8E-2</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -1596,53 +1992,335 @@
         <v>841810</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
-      <c r="G10">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10">
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10">
         <v>1E-3</v>
       </c>
-      <c r="K10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10">
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10">
         <v>100000</v>
       </c>
-      <c r="M10" t="s">
-        <v>53</v>
-      </c>
-      <c r="N10">
+      <c r="N10" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10">
         <v>0.69099999999999995</v>
-      </c>
-      <c r="O10">
-        <v>0.69399999999999995</v>
       </c>
       <c r="P10">
         <v>0.69399999999999995</v>
       </c>
       <c r="Q10">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="R10">
         <v>0.71799999999999997</v>
       </c>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>841840</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11">
+        <v>1E-3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11">
+        <v>100000</v>
+      </c>
+      <c r="N11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O11">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="P11">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="Q11">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="R11">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>841850</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12">
+        <v>10000</v>
+      </c>
+      <c r="N12" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="P12">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="Q12">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="R12">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>841840</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13">
+        <v>100000</v>
+      </c>
+      <c r="N13" t="s">
+        <v>67</v>
+      </c>
+      <c r="O13">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="P13">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="Q13">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="R13">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>841810</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14">
+        <v>42</v>
+      </c>
+      <c r="I14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="L14" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14">
+        <v>50000</v>
+      </c>
+      <c r="N14" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14">
+        <v>0.624</v>
+      </c>
+      <c r="P14">
+        <v>0.66</v>
+      </c>
+      <c r="Q14">
+        <v>0.625</v>
+      </c>
+      <c r="R14">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>841850</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15">
+        <v>1E-3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15">
+        <v>100000</v>
+      </c>
+      <c r="N15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15">
+        <v>0.873</v>
+      </c>
+      <c r="P15">
+        <v>0.874</v>
+      </c>
+      <c r="Q15">
+        <v>0.873</v>
+      </c>
+      <c r="R15">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q10"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>